<commit_message>
Combined sources & corrected C signatures for mix & sources
</commit_message>
<xml_diff>
--- a/Gantt Lake Stable Isotope/Gantt_mussels.xlsx
+++ b/Gantt Lake Stable Isotope/Gantt_mussels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaelynfogelman/Documents/GitHub/Gantt Lake Stable Isotope/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjf0021\Documents\GitHub\Gantt-Stable-Isotope\Gantt Lake Stable Isotope\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD059918-4A9E-224B-9987-1B0A4F38923B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A028E6E2-1005-4E9F-B34E-D67E2FE04F67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="460" windowWidth="25040" windowHeight="14000" xr2:uid="{2608289D-91D8-4842-85D5-AE6F36B1CE03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2608289D-91D8-4842-85D5-AE6F36B1CE03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -48,17 +47,17 @@
     <t>F. escambia</t>
   </si>
   <si>
-    <t>d13N</t>
+    <t>Species</t>
   </si>
   <si>
-    <t>Species</t>
+    <t>d13C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,13 +68,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -105,19 +97,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -437,594 +426,594 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8">
-        <v>-31.41</v>
-      </c>
-      <c r="C2" s="9">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>-30.901849585646296</v>
+      </c>
+      <c r="C2" s="6">
         <v>6.41</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8">
-        <v>-31.9</v>
-      </c>
-      <c r="C3" s="9">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
+        <v>-30.785648109436927</v>
+      </c>
+      <c r="C3" s="6">
         <v>7.25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3">
-        <v>-31.28</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B4" s="1">
+        <v>-30.5038345294879</v>
+      </c>
+      <c r="C4" s="2">
         <v>7.27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1">
-        <v>-31.73</v>
+        <v>-30.097176827060352</v>
       </c>
       <c r="C5" s="2">
         <v>7.76</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1">
-        <v>-31.3</v>
+        <v>-29.884875777540838</v>
       </c>
       <c r="C6" s="2">
         <v>7.65</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="1">
-        <v>-31.2</v>
+        <v>-30.642374802662005</v>
       </c>
       <c r="C7" s="2">
         <v>6.79</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="1">
-        <v>-31.51</v>
+        <v>-30.962949931992885</v>
       </c>
       <c r="C8" s="2">
         <v>7.79</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="1">
-        <v>-31.68</v>
+        <v>-30.591655745345264</v>
       </c>
       <c r="C9" s="2">
         <v>7.46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="1">
-        <v>-31.52</v>
+        <v>-30.633792580221638</v>
       </c>
       <c r="C10" s="2">
         <v>7.47</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="1">
-        <v>-31.66</v>
+        <v>-30.582603648575983</v>
       </c>
       <c r="C11" s="2">
         <v>6.98</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="1">
-        <v>-31.94</v>
+        <v>-30.046714786577475</v>
       </c>
       <c r="C12" s="2">
         <v>7.39</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1">
-        <v>-31.12</v>
+        <v>-30.326307271750728</v>
       </c>
       <c r="C13" s="2">
         <v>7.25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="1">
-        <v>-31.31</v>
+        <v>-30.792331327251823</v>
       </c>
       <c r="C14" s="2">
         <v>7.84</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="1">
-        <v>-31.64</v>
+        <v>-30.916260679954547</v>
       </c>
       <c r="C15" s="2">
         <v>7.23</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="1">
-        <v>-31.35</v>
+        <v>-30.348997880890277</v>
       </c>
       <c r="C16" s="2">
         <v>7.37</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="1">
-        <v>-30.73</v>
+        <v>-30.050189318037663</v>
       </c>
       <c r="C17" s="2">
         <v>6.93</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="1">
-        <v>-30.52</v>
+        <v>-29.971145202129389</v>
       </c>
       <c r="C18" s="2">
         <v>6.92</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
       <c r="B19" s="1">
-        <v>-30.57</v>
+        <v>-30.025605347292579</v>
       </c>
       <c r="C19" s="2">
         <v>6.94</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="1">
-        <v>-30.93</v>
+        <v>-30.244682821863041</v>
       </c>
       <c r="C20" s="2">
         <v>7.09</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="1">
-        <v>-30.64</v>
+        <v>-29.800292992632841</v>
       </c>
       <c r="C21" s="2">
         <v>7.26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="1">
-        <v>-31.77</v>
+        <v>-31.294687529559837</v>
       </c>
       <c r="C22" s="2">
         <v>8.52</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="1">
-        <v>-32.03</v>
+        <v>-31.412815105535344</v>
       </c>
       <c r="C23" s="2">
         <v>8.69</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="1">
-        <v>-32.19</v>
+        <v>-31.479646184952891</v>
       </c>
       <c r="C24" s="2">
         <v>7.89</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
       <c r="B25" s="1">
-        <v>-31.84</v>
+        <v>-31.246585599982655</v>
       </c>
       <c r="C25" s="2">
         <v>7.32</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="1">
-        <v>-32.299999999999997</v>
+        <v>-31.832578715949339</v>
       </c>
       <c r="C26" s="2">
         <v>7.67</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
       <c r="B27" s="1">
-        <v>-30.48</v>
+        <v>-29.913014551693458</v>
       </c>
       <c r="C27" s="2">
         <v>7.05</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="1">
-        <v>-31.1</v>
+        <v>-30.850227884094373</v>
       </c>
       <c r="C28" s="2">
         <v>6.84</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>3</v>
       </c>
       <c r="B29" s="1">
-        <v>-32.15</v>
+        <v>-31.503751406597683</v>
       </c>
       <c r="C29" s="2">
         <v>7.4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="1">
-        <v>-31.81</v>
+        <v>-31.452392077233277</v>
       </c>
       <c r="C30" s="2">
         <v>7.72</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="1">
-        <v>-32.03</v>
+        <v>-31.526191204204604</v>
       </c>
       <c r="C31" s="2">
         <v>7.3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
       <c r="B32" s="1">
-        <v>-31.88</v>
+        <v>-31.388513659501029</v>
       </c>
       <c r="C32" s="2">
         <v>7.18</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
       <c r="B33" s="1">
-        <v>-32.04</v>
+        <v>-31.505393261731264</v>
       </c>
       <c r="C33" s="2">
         <v>7.31</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="1">
-        <v>-31.42</v>
+        <v>-30.790076258516198</v>
       </c>
       <c r="C34" s="2">
         <v>7.09</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>3</v>
       </c>
       <c r="B35" s="1">
-        <v>-31.38</v>
+        <v>-30.91636879160518</v>
       </c>
       <c r="C35" s="2">
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>3</v>
       </c>
       <c r="B36" s="1">
-        <v>-31</v>
+        <v>-30.448443263896458</v>
       </c>
       <c r="C36" s="2">
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>3</v>
       </c>
       <c r="B37" s="1">
-        <v>-31.72</v>
+        <v>-31.407364908381176</v>
       </c>
       <c r="C37" s="2">
         <v>8.65</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>3</v>
       </c>
       <c r="B38" s="1">
-        <v>-31.42</v>
+        <v>-31.092064260620528</v>
       </c>
       <c r="C38" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>3</v>
       </c>
       <c r="B39" s="1">
-        <v>-31.09</v>
+        <v>-30.437175788588597</v>
       </c>
       <c r="C39" s="2">
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>3</v>
       </c>
       <c r="B40" s="1">
-        <v>-31.5</v>
+        <v>-30.724883661706102</v>
       </c>
       <c r="C40" s="2">
         <v>7.36</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>3</v>
       </c>
       <c r="B41" s="1">
-        <v>-31.09</v>
+        <v>-30.689802979886899</v>
       </c>
       <c r="C41" s="2">
         <v>8.5399999999999991</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1</v>
       </c>
       <c r="B42" s="1">
-        <v>-31.03</v>
+        <v>-30.059327853221216</v>
       </c>
       <c r="C42" s="2">
         <v>7.81</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1</v>
       </c>
       <c r="B43" s="1">
-        <v>-31.14</v>
+        <v>-30.668071198638835</v>
       </c>
       <c r="C43" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1</v>
       </c>
       <c r="B44" s="1">
-        <v>-31.43</v>
+        <v>-30.798659795402045</v>
       </c>
       <c r="C44" s="2">
         <v>7.42</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1</v>
       </c>
       <c r="B45" s="1">
-        <v>-31.34</v>
+        <v>-30.787611109446622</v>
       </c>
       <c r="C45" s="2">
         <v>7.93</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1</v>
       </c>
       <c r="B46" s="1">
-        <v>-30.92</v>
+        <v>-30.083324307283526</v>
       </c>
       <c r="C46" s="2">
         <v>7.73</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1</v>
       </c>
       <c r="B47" s="1">
-        <v>-30.96</v>
+        <v>-30.634215805829825</v>
       </c>
       <c r="C47" s="2">
         <v>8.1300000000000008</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1</v>
       </c>
       <c r="B48" s="1">
-        <v>-30.67</v>
+        <v>-30.074407755116685</v>
       </c>
       <c r="C48" s="2">
         <v>7.26</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1</v>
       </c>
       <c r="B49" s="1">
-        <v>-30.97</v>
+        <v>-30.167484895076061</v>
       </c>
       <c r="C49" s="2">
         <v>7.84</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>1</v>
       </c>
       <c r="B50" s="1">
-        <v>-31.52</v>
+        <v>-30.842293734897407</v>
       </c>
       <c r="C50" s="2">
         <v>8.07</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1</v>
       </c>
       <c r="B51" s="1">
-        <v>-31.38</v>
+        <v>-30.83926086978785</v>
       </c>
       <c r="C51" s="2">
         <v>7.87</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>1</v>
       </c>
       <c r="B52" s="1">
-        <v>-31.88</v>
+        <v>-30.93791561306908</v>
       </c>
       <c r="C52" s="2">
         <v>8.01</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="1">
-        <v>-31.33</v>
-      </c>
-      <c r="C53" s="2">
+      <c r="B53">
+        <v>-30.52544128107008</v>
+      </c>
+      <c r="C53">
         <v>7.55</v>
       </c>
     </row>

</xml_diff>